<commit_message>
added saving of optimized program
</commit_message>
<xml_diff>
--- a/logging/datasciencystuff/log_evaluations.xlsx
+++ b/logging/datasciencystuff/log_evaluations.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB11"/>
+  <dimension ref="A1:AB12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5964,6 +5964,108 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>phi3:14b-medium-4k-instruct-q5_K_M</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>llama3:70b</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>42</v>
+      </c>
+      <c r="D12" t="n">
+        <v>200</v>
+      </c>
+      <c r="E12" t="n">
+        <v>2846.55</v>
+      </c>
+      <c r="F12" t="n">
+        <v>306.1151</v>
+      </c>
+      <c r="G12" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>phi3_14b_medium_4k_instruct_q5_K_M_llama3_70b_42_200_val.txt</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
+        <v>477.93</v>
+      </c>
+      <c r="J12" t="n">
+        <v>18.75</v>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>phi3_14b_medium_4k_instruct_q5_K_M_llama3_70b_42_200_test.txt</t>
+        </is>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>4</v>
+      </c>
+      <c r="N12" t="n">
+        <v>148.71</v>
+      </c>
+      <c r="O12" t="n">
+        <v>57.5</v>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>phi3_14b_medium_4k_instruct_q5_K_M_llama3_70b_42_200_val_labeled.txt</t>
+        </is>
+      </c>
+      <c r="Q12" t="n">
+        <v>276.76</v>
+      </c>
+      <c r="R12" t="n">
+        <v>57.5</v>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>phi3_14b_medium_4k_instruct_q5_K_M_llama3_70b_42_200_test_labeled.txt</t>
+        </is>
+      </c>
+      <c r="T12" t="n">
+        <v>1168.15</v>
+      </c>
+      <c r="U12" t="n">
+        <v>2</v>
+      </c>
+      <c r="V12" t="n">
+        <v>2</v>
+      </c>
+      <c r="W12" t="n">
+        <v>133.24</v>
+      </c>
+      <c r="X12" t="n">
+        <v>72.5</v>
+      </c>
+      <c r="Y12" t="inlineStr">
+        <is>
+          <t>phi3_14b_medium_4k_instruct_q5_K_M_llama3_70b_42_200_val_bootstrap.txt</t>
+        </is>
+      </c>
+      <c r="Z12" t="n">
+        <v>335.65</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>52.5</v>
+      </c>
+      <c r="AB12" t="inlineStr">
+        <is>
+          <t>phi3_14b_medium_4k_instruct_q5_K_M_llama3_70b_42_200_test_bootstrap.txt</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>